<commit_message>
update peak correlation on different replicate level (inlab(pseudoreplicates),interlab(across lab and with in lab))
</commit_message>
<xml_diff>
--- a/K562_A549_PeakN.xlsx
+++ b/K562_A549_PeakN.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xindong/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xindong/Downloads/Data_Analysis/cutandrun/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4C0560-7D82-2744-B4D9-DE7FBFEC6D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4668E8C-383A-5044-91E2-FD5F378AD9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28320" windowHeight="20040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>Sample</t>
   </si>
@@ -110,6 +111,15 @@
   </si>
   <si>
     <t>PeakN_Ratio</t>
+  </si>
+  <si>
+    <t>H3K4me3_K562_E4</t>
+  </si>
+  <si>
+    <t>Exp_Name</t>
+  </si>
+  <si>
+    <t>Peak_Number</t>
   </si>
 </sst>
 </file>
@@ -477,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A6" zoomScale="170" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,187 +567,195 @@
         <v>29544</v>
       </c>
       <c r="D6" s="1">
-        <f>B7/B8</f>
+        <f>B8/B9</f>
         <v>3.1501359406044127</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
-        <v>120499</v>
-      </c>
-      <c r="D7" s="1">
-        <f>B10/B11</f>
-        <v>1.2109549038421425</v>
+        <v>43357</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>38252</v>
+        <v>120499</v>
       </c>
       <c r="D8" s="1">
-        <f>B12/B13</f>
-        <v>0.45846802356126115</v>
+        <f>B11/B12</f>
+        <v>1.2109549038421425</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>51343</v>
+        <v>38252</v>
+      </c>
+      <c r="D9" s="1">
+        <f>B13/B14</f>
+        <v>0.45846802356126115</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>145139</v>
+        <v>51343</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>119855</v>
+        <v>145139</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>74176</v>
+        <v>119855</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>74176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <v>161791</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1">
-        <v>124322</v>
-      </c>
-      <c r="D16" s="1">
-        <f>B16/B17</f>
-        <v>0.95572023800372075</v>
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1">
-        <v>130082</v>
+        <v>124322</v>
       </c>
       <c r="D17" s="1">
-        <f>B18/B19</f>
-        <v>0.85712529202016474</v>
+        <f>B17/B18</f>
+        <v>0.95572023800372075</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1">
-        <v>27884</v>
+        <v>130082</v>
       </c>
       <c r="D18" s="1">
-        <f>B21/B22</f>
-        <v>1.593012494215641</v>
+        <f>B19/B20</f>
+        <v>0.85712529202016474</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
-        <v>32532</v>
+        <v>27884</v>
       </c>
       <c r="D19" s="1">
-        <f>B23/B24</f>
-        <v>0.81242526613961152</v>
+        <f>B22/B23</f>
+        <v>1.593012494215641</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1">
-        <v>47957</v>
+        <v>32532</v>
       </c>
       <c r="D20" s="1">
-        <f>B25/B26</f>
-        <v>1.4878544945479204</v>
+        <f>B24/B25</f>
+        <v>0.81242526613961152</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1">
-        <v>75735</v>
+        <v>47957</v>
+      </c>
+      <c r="D21" s="1">
+        <f>B26/B27</f>
+        <v>1.4878544945479204</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1">
-        <v>47542</v>
+        <v>75735</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1">
-        <v>139963</v>
+        <v>47542</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1">
-        <v>172278</v>
+        <v>139963</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1">
-        <v>136039</v>
+        <v>172278</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1">
+        <v>136039</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="2">
         <v>91433</v>
       </c>
     </row>
@@ -745,4 +763,219 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B573A18-3D71-D743-827B-CF27BBAF7BB7}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>112834</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>95383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>21146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>23132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>29544</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>120499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>38252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>51343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>145139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>119855</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>74176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1">
+        <v>161791</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>124322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>130082</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>27884</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>32532</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>47957</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>75735</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>47542</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1">
+        <v>139963</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>172278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>136039</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>91433</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>